<commit_message>
20250812 WIFRP INcl Excl
</commit_message>
<xml_diff>
--- a/GUI + Reviews/Structure Review Tool.xlsx
+++ b/GUI + Reviews/Structure Review Tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{790FDA62-ACCA-4293-82A4-A97B907B6C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5D34C0D-813C-4528-ACB2-F8A1DFD3E3CA}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{790FDA62-ACCA-4293-82A4-A97B907B6C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD4AF31D-199F-4068-981B-38477456D6E9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE21F411-BF57-48EB-A8D8-A2241EE09945}"/>
+    <workbookView xWindow="-29370" yWindow="195" windowWidth="29040" windowHeight="15720" xr2:uid="{FE21F411-BF57-48EB-A8D8-A2241EE09945}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>aexew_review</t>
   </si>
   <si>
-    <t>be1p_review</t>
-  </si>
-  <si>
-    <t>bnew_review</t>
-  </si>
-  <si>
     <t>Helper functions</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>Script</t>
   </si>
   <si>
-    <t>Inclusion Exclusion</t>
-  </si>
-  <si>
     <t>Configuration Files</t>
   </si>
   <si>
@@ -117,16 +108,37 @@
   </si>
   <si>
     <t>Sheet</t>
+  </si>
+  <si>
+    <t>Inclusion Exclusion Logic</t>
+  </si>
+  <si>
+    <t>wifrp_review</t>
+  </si>
+  <si>
+    <t>edwpt_review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C5700"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -137,13 +149,37 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF9C5700"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -192,21 +228,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1124,114 +1170,115 @@
   <dimension ref="F2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="6" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="6:10" x14ac:dyDescent="0.2">
       <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="6:10" x14ac:dyDescent="0.2">
       <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="J8" s="14" t="s">
         <v>4</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="J8" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F9" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F10" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="H14" s="5" t="s">
-        <v>24</v>
+      <c r="H14" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="6:10" x14ac:dyDescent="0.2">
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="8:12" x14ac:dyDescent="0.2">
-      <c r="H17" s="2" t="s">
-        <v>2</v>
+      <c r="H17" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.2">
-      <c r="H18" s="2" t="s">
-        <v>3</v>
+      <c r="H18" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="8:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H19" s="3" t="s">
-        <v>9</v>
+      <c r="H19" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="8:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H23" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="8:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1239,28 +1286,28 @@
     </row>
     <row r="25" spans="8:12" x14ac:dyDescent="0.2">
       <c r="J25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="8:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H27" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="8:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H28" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>